<commit_message>
Other search comparison files
</commit_message>
<xml_diff>
--- a/searchterms.xlsx
+++ b/searchterms.xlsx
@@ -24,34 +24,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>hiv</t>
   </si>
   <si>
-    <t>std</t>
-  </si>
-  <si>
-    <t>colon cancer</t>
-  </si>
-  <si>
-    <t>bananas</t>
-  </si>
-  <si>
-    <t>Zika</t>
+    <t>zika</t>
+  </si>
+  <si>
+    <t>flu</t>
+  </si>
+  <si>
+    <t>influenza</t>
+  </si>
+  <si>
+    <t>vis</t>
+  </si>
+  <si>
+    <t>malaria</t>
+  </si>
+  <si>
+    <t>hpv</t>
+  </si>
+  <si>
+    <t>ebola</t>
+  </si>
+  <si>
+    <t>diabetes</t>
+  </si>
+  <si>
+    <t>hepatitis b</t>
+  </si>
+  <si>
+    <t>tuberculosis</t>
+  </si>
+  <si>
+    <t>obesity</t>
+  </si>
+  <si>
+    <t>vaccines</t>
+  </si>
+  <si>
+    <t>chlamydia</t>
+  </si>
+  <si>
+    <t>immunization schedule 2017</t>
+  </si>
+  <si>
+    <t>zika virus</t>
+  </si>
+  <si>
+    <t>influenza 2017</t>
+  </si>
+  <si>
+    <t>measles</t>
+  </si>
+  <si>
+    <t>mumps</t>
+  </si>
+  <si>
+    <t>rabies</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -62,7 +113,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,12 +121,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -356,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,32 +434,108 @@
     <col min="1" max="1" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
+    <row r="6" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>